<commit_message>
Doku: Archivische Ablieferungsschnittstelle Stand 2014-08-14
</commit_message>
<xml_diff>
--- a/documentation_xml_lang_de.xlsx
+++ b/documentation_xml_lang_de.xlsx
@@ -14,7 +14,10 @@
   <sheets>
     <sheet name="documentation_xml_lang_de" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">documentation_xml_lang_de!$A$1:$C$128</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -700,7 +703,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -830,6 +833,126 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -875,7 +998,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -883,10 +1006,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1210,1044 +1360,2237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B128"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C128" sqref="A1:C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="160.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="3.875" customWidth="1"/>
+    <col min="3" max="3" width="160.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="C2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="C3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="C4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="C5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="C6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="C7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="C8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="C9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="C10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5">
+        <v>11</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5">
+        <v>12</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5">
+        <v>13</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5">
+        <v>14</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="5">
+        <v>15</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5">
+        <v>16</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5">
+        <v>17</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5">
+        <v>18</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="5">
+        <v>19</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5">
+        <v>20</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="5">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="C21" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="5">
+        <v>22</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="5">
+        <v>23</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="5">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="C24" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="5">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="C25" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="C26" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="5">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="C27" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="5">
+        <v>28</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="5">
+        <v>29</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="5">
+        <v>30</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="5">
+        <v>31</v>
+      </c>
+      <c r="C31" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="5">
+        <v>32</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="5">
+        <v>33</v>
+      </c>
+      <c r="C33" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="5">
+        <v>34</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="5">
+        <v>35</v>
+      </c>
+      <c r="C35" s="10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="5">
+        <v>36</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="5">
+        <v>37</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="5">
+        <v>38</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="5">
+        <v>39</v>
+      </c>
+      <c r="C39" s="10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="5">
+        <v>40</v>
+      </c>
+      <c r="C40" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="5">
+        <v>41</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="5">
+        <v>42</v>
+      </c>
+      <c r="C42" s="10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="5">
+        <v>43</v>
+      </c>
+      <c r="C43" s="10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="5">
+        <v>44</v>
+      </c>
+      <c r="C44" s="10" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="5">
+        <v>45</v>
+      </c>
+      <c r="C45" s="10" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="5">
+        <v>46</v>
+      </c>
+      <c r="C46" s="10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="5">
+        <v>47</v>
+      </c>
+      <c r="C47" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="5">
+        <v>48</v>
+      </c>
+      <c r="C48" s="10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="5">
+        <v>49</v>
+      </c>
+      <c r="C49" s="10" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A50" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="5">
+        <v>50</v>
+      </c>
+      <c r="C50" s="10" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="5">
+        <v>51</v>
+      </c>
+      <c r="C51" s="10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="5">
+        <v>52</v>
+      </c>
+      <c r="C52" s="10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="5">
+        <v>53</v>
+      </c>
+      <c r="C53" s="10" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A54" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="5">
+        <v>54</v>
+      </c>
+      <c r="C54" s="10" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="5">
+        <v>55</v>
+      </c>
+      <c r="C55" s="10" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
+      <c r="D55" s="3"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="5">
+        <v>56</v>
+      </c>
+      <c r="C56" s="10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A57" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="5">
+        <v>57</v>
+      </c>
+      <c r="C57" s="10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="5">
+        <v>58</v>
+      </c>
+      <c r="C58" s="10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="5">
+        <v>59</v>
+      </c>
+      <c r="C59" s="10" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="5">
+        <v>60</v>
+      </c>
+      <c r="C60" s="10" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="5">
+        <v>61</v>
+      </c>
+      <c r="C61" s="10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="5">
+        <v>62</v>
+      </c>
+      <c r="C62" s="10" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="5">
+        <v>63</v>
+      </c>
+      <c r="C63" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A64" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="5">
+        <v>64</v>
+      </c>
+      <c r="C64" s="10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
+      <c r="D64" s="3"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="5">
+        <v>65</v>
+      </c>
+      <c r="C65" s="10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
+      <c r="D65" s="3"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="5">
+        <v>66</v>
+      </c>
+      <c r="C66" s="10" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
+      <c r="D66" s="3"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="5">
+        <v>67</v>
+      </c>
+      <c r="C67" s="10" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
+      <c r="D67" s="3"/>
+    </row>
+    <row r="68" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="5">
+        <v>68</v>
+      </c>
+      <c r="C68" s="10" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
+      <c r="D68" s="3"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="5">
+        <v>69</v>
+      </c>
+      <c r="C69" s="10" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="3" t="s">
+      <c r="D69" s="3"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="5">
+        <v>70</v>
+      </c>
+      <c r="C70" s="10" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
+      <c r="D70" s="3"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="5">
+        <v>71</v>
+      </c>
+      <c r="C71" s="10" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A72" s="3" t="s">
+      <c r="D71" s="3"/>
+    </row>
+    <row r="72" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A72" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="5">
+        <v>72</v>
+      </c>
+      <c r="C72" s="10" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A73" s="3" t="s">
+      <c r="D72" s="3"/>
+    </row>
+    <row r="73" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A73" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="5">
+        <v>73</v>
+      </c>
+      <c r="C73" s="10" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A74" s="3" t="s">
+      <c r="D73" s="3"/>
+    </row>
+    <row r="74" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A74" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="5">
+        <v>74</v>
+      </c>
+      <c r="C74" s="10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A75" s="3" t="s">
+      <c r="D74" s="3"/>
+    </row>
+    <row r="75" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A75" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="5">
+        <v>75</v>
+      </c>
+      <c r="C75" s="10" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A76" s="3" t="s">
+      <c r="D75" s="3"/>
+    </row>
+    <row r="76" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A76" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="5">
+        <v>76</v>
+      </c>
+      <c r="C76" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
+      <c r="D76" s="3"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="5">
+        <v>77</v>
+      </c>
+      <c r="C77" s="10" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="3" t="s">
+      <c r="D77" s="3"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="5">
+        <v>78</v>
+      </c>
+      <c r="C78" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
+      <c r="D78" s="3"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="5">
+        <v>79</v>
+      </c>
+      <c r="C79" s="10" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="3" t="s">
+      <c r="D79" s="3"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="5">
+        <v>80</v>
+      </c>
+      <c r="C80" s="10" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
+      <c r="D80" s="3"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="5">
+        <v>81</v>
+      </c>
+      <c r="C81" s="10" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
+      <c r="D81" s="3"/>
+    </row>
+    <row r="82" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A82" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="5">
+        <v>82</v>
+      </c>
+      <c r="C82" s="10" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
+      <c r="D82" s="3"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="5">
+        <v>83</v>
+      </c>
+      <c r="C83" s="10" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
+      <c r="D83" s="3"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="5">
+        <v>84</v>
+      </c>
+      <c r="C84" s="10" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
+      <c r="D84" s="3"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="5">
+        <v>85</v>
+      </c>
+      <c r="C85" s="10" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
+      <c r="D85" s="3"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="5">
+        <v>86</v>
+      </c>
+      <c r="C86" s="10" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
+      <c r="D86" s="3"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="5">
+        <v>87</v>
+      </c>
+      <c r="C87" s="10" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
+      <c r="D87" s="3"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="5">
+        <v>88</v>
+      </c>
+      <c r="C88" s="10" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
+      <c r="D88" s="3"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="5">
+        <v>89</v>
+      </c>
+      <c r="C89" s="10" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
+      <c r="D89" s="3"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="5">
+        <v>90</v>
+      </c>
+      <c r="C90" s="10" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
+      <c r="D90" s="3"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="5">
+        <v>91</v>
+      </c>
+      <c r="C91" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="3" t="s">
+      <c r="D91" s="3"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B92" s="5">
+        <v>92</v>
+      </c>
+      <c r="C92" s="10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
+      <c r="D92" s="3"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B93" s="5">
+        <v>93</v>
+      </c>
+      <c r="C93" s="10" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
+      <c r="D93" s="3"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="5">
+        <v>94</v>
+      </c>
+      <c r="C94" s="10" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="3" t="s">
+      <c r="D94" s="3"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="5">
+        <v>95</v>
+      </c>
+      <c r="C95" s="10" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
+      <c r="D95" s="3"/>
+    </row>
+    <row r="96" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A96" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="5">
+        <v>96</v>
+      </c>
+      <c r="C96" s="10" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
+      <c r="D96" s="3"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B97" s="5">
+        <v>97</v>
+      </c>
+      <c r="C97" s="10" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="3" t="s">
+      <c r="D97" s="3"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B98" s="5">
+        <v>98</v>
+      </c>
+      <c r="C98" s="10" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="3" t="s">
+      <c r="D98" s="3"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B99" s="5">
+        <v>99</v>
+      </c>
+      <c r="C99" s="10" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="3" t="s">
+      <c r="D99" s="3"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B100" s="5">
+        <v>100</v>
+      </c>
+      <c r="C100" s="10" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="3" t="s">
+      <c r="D100" s="3"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B101" s="5">
+        <v>101</v>
+      </c>
+      <c r="C101" s="10" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="3" t="s">
+      <c r="D101" s="3"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B102" s="5">
+        <v>102</v>
+      </c>
+      <c r="C102" s="10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" s="3" t="s">
+      <c r="D102" s="3"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B103" s="5">
+        <v>103</v>
+      </c>
+      <c r="C103" s="10" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A104" s="3" t="s">
+      <c r="D103" s="3"/>
+    </row>
+    <row r="104" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A104" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B104" s="5">
+        <v>104</v>
+      </c>
+      <c r="C104" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A105" s="3" t="s">
+      <c r="D104" s="3"/>
+    </row>
+    <row r="105" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A105" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B105" s="5">
+        <v>105</v>
+      </c>
+      <c r="C105" s="10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A106" s="3" t="s">
+      <c r="D105" s="3"/>
+    </row>
+    <row r="106" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A106" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B106" s="5">
+        <v>106</v>
+      </c>
+      <c r="C106" s="10" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A107" s="3" t="s">
+      <c r="D106" s="3"/>
+    </row>
+    <row r="107" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A107" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B107" s="5">
+        <v>107</v>
+      </c>
+      <c r="C107" s="10" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="3" t="s">
+      <c r="D107" s="3"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B108" s="5">
+        <v>108</v>
+      </c>
+      <c r="C108" s="10" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="3" t="s">
+      <c r="D108" s="3"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B109" s="5">
+        <v>109</v>
+      </c>
+      <c r="C109" s="10" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="3" t="s">
+      <c r="D109" s="3"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B110" s="5">
+        <v>110</v>
+      </c>
+      <c r="C110" s="10" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="3" t="s">
+      <c r="D110" s="3"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B111" s="5">
+        <v>111</v>
+      </c>
+      <c r="C111" s="10" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="3" t="s">
+      <c r="D111" s="3"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B112" s="5">
+        <v>112</v>
+      </c>
+      <c r="C112" s="10" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="3" t="s">
+      <c r="D112" s="3"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B113" s="5">
+        <v>113</v>
+      </c>
+      <c r="C113" s="10" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="3" t="s">
+      <c r="D113" s="3"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B114" s="5">
+        <v>114</v>
+      </c>
+      <c r="C114" s="10" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="3" t="s">
+      <c r="D114" s="3"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B115" s="5">
+        <v>115</v>
+      </c>
+      <c r="C115" s="10" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" s="3" t="s">
+      <c r="D115" s="3"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B116" s="5">
+        <v>116</v>
+      </c>
+      <c r="C116" s="10" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="3" t="s">
+      <c r="D116" s="3"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B117" s="5">
+        <v>117</v>
+      </c>
+      <c r="C117" s="10" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" s="3" t="s">
+      <c r="D117" s="3"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B118" s="5">
+        <v>118</v>
+      </c>
+      <c r="C118" s="10" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A119" s="3" t="s">
+      <c r="D118" s="3"/>
+    </row>
+    <row r="119" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A119" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B119" s="5">
+        <v>119</v>
+      </c>
+      <c r="C119" s="10" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" s="3" t="s">
+      <c r="D119" s="3"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B120" s="5">
+        <v>120</v>
+      </c>
+      <c r="C120" s="10" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A121" s="3" t="s">
+      <c r="D120" s="3"/>
+    </row>
+    <row r="121" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A121" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B121" s="5">
+        <v>121</v>
+      </c>
+      <c r="C121" s="10" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A122" s="3" t="s">
+      <c r="D121" s="3"/>
+    </row>
+    <row r="122" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A122" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B122" s="5">
+        <v>122</v>
+      </c>
+      <c r="C122" s="10" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A123" s="3" t="s">
+      <c r="D122" s="3"/>
+    </row>
+    <row r="123" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A123" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B123" s="5">
+        <v>123</v>
+      </c>
+      <c r="C123" s="10" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A124" s="3" t="s">
+      <c r="D123" s="3"/>
+    </row>
+    <row r="124" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A124" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B124" s="5">
+        <v>124</v>
+      </c>
+      <c r="C124" s="10" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="3" t="s">
+      <c r="D124" s="3"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="B125" s="5">
+        <v>125</v>
+      </c>
+      <c r="C125" s="10" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="3" t="s">
+      <c r="D125" s="3"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="B126" s="5">
+        <v>126</v>
+      </c>
+      <c r="C126" s="10" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="3" t="s">
+      <c r="D126" s="3"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B127" s="5">
+        <v>127</v>
+      </c>
+      <c r="C127" s="10" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" s="3" t="s">
+      <c r="D127" s="3"/>
+    </row>
+    <row r="128" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B128" s="12">
+        <v>128</v>
+      </c>
+      <c r="C128" s="13" t="s">
         <v>124</v>
       </c>
+      <c r="D128" s="3"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="4"/>
+      <c r="B129" s="4"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="4"/>
+      <c r="B130" s="4"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="4"/>
+      <c r="B131" s="4"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="4"/>
+      <c r="B132" s="4"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="4"/>
+      <c r="B133" s="4"/>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="4"/>
+      <c r="B134" s="4"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="4"/>
+      <c r="B135" s="4"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="4"/>
+      <c r="B136" s="4"/>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="4"/>
+      <c r="B137" s="4"/>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="4"/>
+      <c r="B138" s="4"/>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="4"/>
+      <c r="B139" s="4"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="4"/>
+      <c r="B140" s="4"/>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="4"/>
+      <c r="B141" s="4"/>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="4"/>
+      <c r="B142" s="4"/>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="4"/>
+      <c r="B143" s="4"/>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="4"/>
+      <c r="B144" s="4"/>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="4"/>
+      <c r="B145" s="4"/>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="4"/>
+      <c r="B146" s="4"/>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="4"/>
+      <c r="B147" s="4"/>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="4"/>
+      <c r="B148" s="4"/>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="4"/>
+      <c r="B149" s="4"/>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="4"/>
+      <c r="B150" s="4"/>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="4"/>
+      <c r="B151" s="4"/>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="4"/>
+      <c r="B152" s="4"/>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="4"/>
+      <c r="B153" s="4"/>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="4"/>
+      <c r="B154" s="4"/>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="4"/>
+      <c r="B155" s="4"/>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="4"/>
+      <c r="B156" s="4"/>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="4"/>
+      <c r="B157" s="4"/>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="4"/>
+      <c r="B158" s="4"/>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="4"/>
+      <c r="B159" s="4"/>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="4"/>
+      <c r="B160" s="4"/>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="4"/>
+      <c r="B161" s="4"/>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="4"/>
+      <c r="B162" s="4"/>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="4"/>
+      <c r="B163" s="4"/>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="4"/>
+      <c r="B164" s="4"/>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" s="4"/>
+      <c r="B165" s="4"/>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="4"/>
+      <c r="B166" s="4"/>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="4"/>
+      <c r="B167" s="4"/>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="4"/>
+      <c r="B168" s="4"/>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" s="4"/>
+      <c r="B169" s="4"/>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" s="4"/>
+      <c r="B170" s="4"/>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" s="4"/>
+      <c r="B171" s="4"/>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" s="4"/>
+      <c r="B172" s="4"/>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" s="4"/>
+      <c r="B173" s="4"/>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" s="4"/>
+      <c r="B174" s="4"/>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" s="4"/>
+      <c r="B175" s="4"/>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" s="4"/>
+      <c r="B176" s="4"/>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="4"/>
+      <c r="B177" s="4"/>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="4"/>
+      <c r="B178" s="4"/>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" s="4"/>
+      <c r="B179" s="4"/>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="4"/>
+      <c r="B180" s="4"/>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="4"/>
+      <c r="B181" s="4"/>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" s="4"/>
+      <c r="B182" s="4"/>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" s="4"/>
+      <c r="B183" s="4"/>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" s="4"/>
+      <c r="B184" s="4"/>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" s="4"/>
+      <c r="B185" s="4"/>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" s="4"/>
+      <c r="B186" s="4"/>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187" s="4"/>
+      <c r="B187" s="4"/>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" s="4"/>
+      <c r="B188" s="4"/>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" s="4"/>
+      <c r="B189" s="4"/>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" s="4"/>
+      <c r="B190" s="4"/>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191" s="4"/>
+      <c r="B191" s="4"/>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192" s="4"/>
+      <c r="B192" s="4"/>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193" s="4"/>
+      <c r="B193" s="4"/>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" s="4"/>
+      <c r="B194" s="4"/>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" s="4"/>
+      <c r="B195" s="4"/>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" s="4"/>
+      <c r="B196" s="4"/>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" s="4"/>
+      <c r="B197" s="4"/>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" s="4"/>
+      <c r="B198" s="4"/>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" s="4"/>
+      <c r="B199" s="4"/>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" s="4"/>
+      <c r="B200" s="4"/>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" s="4"/>
+      <c r="B201" s="4"/>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" s="4"/>
+      <c r="B202" s="4"/>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" s="4"/>
+      <c r="B203" s="4"/>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" s="4"/>
+      <c r="B204" s="4"/>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205" s="4"/>
+      <c r="B205" s="4"/>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206" s="4"/>
+      <c r="B206" s="4"/>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207" s="4"/>
+      <c r="B207" s="4"/>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208" s="4"/>
+      <c r="B208" s="4"/>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209" s="4"/>
+      <c r="B209" s="4"/>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210" s="4"/>
+      <c r="B210" s="4"/>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A211" s="4"/>
+      <c r="B211" s="4"/>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A212" s="4"/>
+      <c r="B212" s="4"/>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A213" s="4"/>
+      <c r="B213" s="4"/>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A214" s="4"/>
+      <c r="B214" s="4"/>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A215" s="4"/>
+      <c r="B215" s="4"/>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A216" s="4"/>
+      <c r="B216" s="4"/>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A217" s="4"/>
+      <c r="B217" s="4"/>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218" s="4"/>
+      <c r="B218" s="4"/>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A219" s="4"/>
+      <c r="B219" s="4"/>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220" s="4"/>
+      <c r="B220" s="4"/>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221" s="4"/>
+      <c r="B221" s="4"/>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222" s="4"/>
+      <c r="B222" s="4"/>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223" s="4"/>
+      <c r="B223" s="4"/>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224" s="4"/>
+      <c r="B224" s="4"/>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A225" s="4"/>
+      <c r="B225" s="4"/>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A226" s="4"/>
+      <c r="B226" s="4"/>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A227" s="4"/>
+      <c r="B227" s="4"/>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A228" s="4"/>
+      <c r="B228" s="4"/>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A229" s="4"/>
+      <c r="B229" s="4"/>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A230" s="4"/>
+      <c r="B230" s="4"/>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A231" s="4"/>
+      <c r="B231" s="4"/>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A232" s="4"/>
+      <c r="B232" s="4"/>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A233" s="4"/>
+      <c r="B233" s="4"/>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A234" s="4"/>
+      <c r="B234" s="4"/>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A235" s="4"/>
+      <c r="B235" s="4"/>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A236" s="4"/>
+      <c r="B236" s="4"/>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A237" s="4"/>
+      <c r="B237" s="4"/>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A238" s="4"/>
+      <c r="B238" s="4"/>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A239" s="4"/>
+      <c r="B239" s="4"/>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A240" s="4"/>
+      <c r="B240" s="4"/>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A241" s="4"/>
+      <c r="B241" s="4"/>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A242" s="4"/>
+      <c r="B242" s="4"/>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A243" s="4"/>
+      <c r="B243" s="4"/>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A244" s="4"/>
+      <c r="B244" s="4"/>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A245" s="4"/>
+      <c r="B245" s="4"/>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A246" s="4"/>
+      <c r="B246" s="4"/>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A247" s="4"/>
+      <c r="B247" s="4"/>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A248" s="4"/>
+      <c r="B248" s="4"/>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A249" s="4"/>
+      <c r="B249" s="4"/>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A250" s="4"/>
+      <c r="B250" s="4"/>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A251" s="4"/>
+      <c r="B251" s="4"/>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A252" s="4"/>
+      <c r="B252" s="4"/>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A253" s="4"/>
+      <c r="B253" s="4"/>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A254" s="4"/>
+      <c r="B254" s="4"/>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A255" s="4"/>
+      <c r="B255" s="4"/>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A256" s="4"/>
+      <c r="B256" s="4"/>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A257" s="4"/>
+      <c r="B257" s="4"/>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A258" s="4"/>
+      <c r="B258" s="4"/>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A259" s="4"/>
+      <c r="B259" s="4"/>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A260" s="4"/>
+      <c r="B260" s="4"/>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A261" s="4"/>
+      <c r="B261" s="4"/>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A262" s="4"/>
+      <c r="B262" s="4"/>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A263" s="4"/>
+      <c r="B263" s="4"/>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A264" s="4"/>
+      <c r="B264" s="4"/>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A265" s="4"/>
+      <c r="B265" s="4"/>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A266" s="4"/>
+      <c r="B266" s="4"/>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A267" s="4"/>
+      <c r="B267" s="4"/>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A268" s="4"/>
+      <c r="B268" s="4"/>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A269" s="4"/>
+      <c r="B269" s="4"/>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A270" s="4"/>
+      <c r="B270" s="4"/>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A271" s="4"/>
+      <c r="B271" s="4"/>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A272" s="4"/>
+      <c r="B272" s="4"/>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A273" s="4"/>
+      <c r="B273" s="4"/>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A274" s="4"/>
+      <c r="B274" s="4"/>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A275" s="4"/>
+      <c r="B275" s="4"/>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A276" s="4"/>
+      <c r="B276" s="4"/>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A277" s="4"/>
+      <c r="B277" s="4"/>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A278" s="4"/>
+      <c r="B278" s="4"/>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A279" s="4"/>
+      <c r="B279" s="4"/>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A280" s="4"/>
+      <c r="B280" s="4"/>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A281" s="4"/>
+      <c r="B281" s="4"/>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A282" s="4"/>
+      <c r="B282" s="4"/>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A283" s="4"/>
+      <c r="B283" s="4"/>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A284" s="4"/>
+      <c r="B284" s="4"/>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A285" s="4"/>
+      <c r="B285" s="4"/>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A286" s="4"/>
+      <c r="B286" s="4"/>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A287" s="4"/>
+      <c r="B287" s="4"/>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A288" s="4"/>
+      <c r="B288" s="4"/>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A289" s="4"/>
+      <c r="B289" s="4"/>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A290" s="4"/>
+      <c r="B290" s="4"/>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A291" s="4"/>
+      <c r="B291" s="4"/>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A292" s="4"/>
+      <c r="B292" s="4"/>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A293" s="4"/>
+      <c r="B293" s="4"/>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A294" s="4"/>
+      <c r="B294" s="4"/>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A295" s="4"/>
+      <c r="B295" s="4"/>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A296" s="4"/>
+      <c r="B296" s="4"/>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A297" s="4"/>
+      <c r="B297" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="81" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>